<commit_message>
25.06.2023 mybee end rewrite
</commit_message>
<xml_diff>
--- a/2tecnolog/ONTP.xlsx
+++ b/2tecnolog/ONTP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreyA\Desktop\Сессия\DIPLOM\2tecnolog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E104A3E-DBF1-4881-8F91-4A4EBBDAD363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0F4686-887D-4A5E-93A1-A7DA668FA9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" firstSheet="13" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="869" firstSheet="14" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tab_1" sheetId="12" r:id="rId1"/>
@@ -5024,7 +5024,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>110</v>
       </c>
@@ -6315,8 +6315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934986B0-5EE4-4C77-A32F-26A1E7F2317A}">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D14"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6638,13 +6638,13 @@
         <v>8</v>
       </c>
       <c r="D10" s="75">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E10" s="70">
         <v>8</v>
       </c>
       <c r="F10" s="75">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="I10" s="69" t="s">
         <v>290</v>
@@ -6676,13 +6676,13 @@
         <v>92</v>
       </c>
       <c r="D11" s="76">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E11" s="70">
         <v>92</v>
       </c>
       <c r="F11" s="76">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="I11" s="69" t="s">
         <v>291</v>
@@ -6776,7 +6776,7 @@
         <v>5</v>
       </c>
       <c r="F14" s="75">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I14" s="69" t="s">
         <v>292</v>
@@ -6814,7 +6814,7 @@
         <v>95</v>
       </c>
       <c r="F15" s="76">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="I15" s="69" t="s">
         <v>291</v>
@@ -8543,7 +8543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6BEE19-31FB-4DCE-83A5-DE13D6D280B1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -8568,7 +8570,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M4"/>
+      <selection activeCell="B2" sqref="B2:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9131,7 +9133,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9435,8 +9437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7EB7266-5EF9-4E07-8BA0-B2CCE59CEA3F}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10086,7 +10088,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="62" t="s">
         <v>545</v>
@@ -10242,7 +10244,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="62" t="s">
         <v>378</v>
@@ -10320,7 +10322,7 @@
         <v>9</v>
       </c>
       <c r="E27" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="62" t="s">
         <v>380</v>
@@ -10389,7 +10391,7 @@
         <v>379</v>
       </c>
       <c r="B29" s="46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="46">
         <v>18</v>
@@ -10398,7 +10400,7 @@
         <v>12</v>
       </c>
       <c r="E29" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="63" t="s">
         <v>547</v>
@@ -10474,7 +10476,7 @@
         <v>551</v>
       </c>
       <c r="B32" s="46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="27">
         <v>30</v>

</xml_diff>